<commit_message>
get question and answers
</commit_message>
<xml_diff>
--- a/ExamToeicOnline-BackEnd-Clients/ExamToeicOnline-BackEnd-Clients/File/Exam01/Đề số 01.xlsx
+++ b/ExamToeicOnline-BackEnd-Clients/ExamToeicOnline-BackEnd-Clients/File/Exam01/Đề số 01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam 4\HK I\TLCN\TLCN\ExamToeicOnline-BackEnd-Clients\ExamToeicOnline-BackEnd-Clients\File\Exam02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA5B956-86E4-41EC-BF30-2D034D4E0A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9671E96F-6DAD-4C58-832C-07430E45F964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="9" r:id="rId1"/>
@@ -27,12 +27,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Part 6'!$B$1:$B$81</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Part 7'!$A$1:$E$271</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="853">
   <si>
     <t>35. What does the woman say a town recently did?</t>
   </si>
@@ -2588,13 +2588,16 @@
   </si>
   <si>
     <t>D. To explain a policy change</t>
+  </si>
+  <si>
+    <t>Correct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2692,6 +2695,14 @@
       <sz val="10"/>
       <name val="Calibri "/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2757,9 +2768,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2783,6 +2791,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3100,8 +3111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF89FB1-9491-4D31-A4C6-DCB09EA1A419}">
   <dimension ref="B1:C31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3118,155 +3129,157 @@
       <c r="B1" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="23" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="2" spans="2:3" ht="14.4">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="14.4">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="14.4">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.4">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="21" spans="2:2">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="14.4">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="19" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="19" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="14.4">
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="19" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="29" spans="2:2">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
         <v>334</v>
       </c>
     </row>
@@ -6454,234 +6467,234 @@
       <c r="B1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="13.8">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="13.8">
-      <c r="A3" s="16"/>
-      <c r="B3" s="18" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="13.8">
-      <c r="A4" s="16"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5" ht="13.8">
-      <c r="A5" s="16"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="17" t="s">
         <v>509</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5" ht="13.8">
-      <c r="A6" s="16"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="17" t="s">
         <v>510</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="13.8">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16" t="s">
         <v>511</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" ht="13.8">
-      <c r="A8" s="16"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="17" t="s">
         <v>512</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" ht="13.8">
-      <c r="A9" s="16"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="17" t="s">
         <v>513</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" ht="13.8">
-      <c r="A10" s="16"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="17" t="s">
         <v>514</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:5" ht="13.8">
-      <c r="A11" s="16"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="13.8">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16" t="s">
         <v>516</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" ht="13.8">
-      <c r="A13" s="16"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5" ht="13.8">
-      <c r="A14" s="16"/>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:5" ht="13.8">
-      <c r="A15" s="16"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="17" t="s">
         <v>519</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" ht="13.8">
-      <c r="A16" s="16"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="17" t="s">
         <v>520</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="13.8">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16" t="s">
         <v>521</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" ht="13.8">
-      <c r="A18" s="16"/>
-      <c r="B18" s="18" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17" t="s">
         <v>522</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="13.8">
-      <c r="A19" s="16"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="17" t="s">
         <v>523</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" ht="13.8">
-      <c r="A20" s="16"/>
-      <c r="B20" s="18" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="17" t="s">
         <v>524</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="17" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="17" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="17" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="31" spans="1:5" customFormat="1">
       <c r="A31" s="3"/>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>535</v>
       </c>
       <c r="D31" s="3"/>
@@ -6689,7 +6702,7 @@
     </row>
     <row r="32" spans="1:5" customFormat="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>536</v>
       </c>
       <c r="D32" s="3"/>
@@ -6697,7 +6710,7 @@
     </row>
     <row r="33" spans="1:5" customFormat="1" ht="26.4">
       <c r="A33" s="3"/>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>537</v>
       </c>
       <c r="D33" s="3"/>
@@ -6705,7 +6718,7 @@
     </row>
     <row r="34" spans="1:5" customFormat="1">
       <c r="A34" s="3"/>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>538</v>
       </c>
       <c r="D34" s="3"/>
@@ -6713,7 +6726,7 @@
     </row>
     <row r="35" spans="1:5" customFormat="1">
       <c r="A35" s="3"/>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>539</v>
       </c>
       <c r="D35" s="3"/>
@@ -6721,7 +6734,7 @@
     </row>
     <row r="36" spans="1:5" customFormat="1">
       <c r="A36" s="3"/>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="17" t="s">
         <v>540</v>
       </c>
       <c r="D36" s="3"/>
@@ -6729,7 +6742,7 @@
     </row>
     <row r="37" spans="1:5" customFormat="1">
       <c r="A37" s="3"/>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>541</v>
       </c>
       <c r="D37" s="3"/>
@@ -6737,7 +6750,7 @@
     </row>
     <row r="38" spans="1:5" customFormat="1">
       <c r="A38" s="3"/>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="17" t="s">
         <v>542</v>
       </c>
       <c r="D38" s="3"/>
@@ -6745,7 +6758,7 @@
     </row>
     <row r="39" spans="1:5" customFormat="1">
       <c r="A39" s="3"/>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="17" t="s">
         <v>543</v>
       </c>
       <c r="D39" s="3"/>
@@ -6753,7 +6766,7 @@
     </row>
     <row r="40" spans="1:5" customFormat="1">
       <c r="A40" s="3"/>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="17" t="s">
         <v>544</v>
       </c>
       <c r="D40" s="3"/>
@@ -6761,7 +6774,7 @@
     </row>
     <row r="41" spans="1:5" customFormat="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="17" t="s">
         <v>545</v>
       </c>
       <c r="D41" s="3"/>
@@ -6769,7 +6782,7 @@
     </row>
     <row r="42" spans="1:5" customFormat="1">
       <c r="A42" s="3"/>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="16" t="s">
         <v>546</v>
       </c>
       <c r="D42" s="3"/>
@@ -6777,7 +6790,7 @@
     </row>
     <row r="43" spans="1:5" customFormat="1">
       <c r="A43" s="3"/>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="17" t="s">
         <v>547</v>
       </c>
       <c r="D43" s="3"/>
@@ -6785,7 +6798,7 @@
     </row>
     <row r="44" spans="1:5" customFormat="1">
       <c r="A44" s="3"/>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="17" t="s">
         <v>548</v>
       </c>
       <c r="D44" s="3"/>
@@ -6793,7 +6806,7 @@
     </row>
     <row r="45" spans="1:5" customFormat="1">
       <c r="A45" s="3"/>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="17" t="s">
         <v>549</v>
       </c>
       <c r="D45" s="3"/>
@@ -6801,7 +6814,7 @@
     </row>
     <row r="46" spans="1:5" customFormat="1">
       <c r="A46" s="3"/>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="17" t="s">
         <v>550</v>
       </c>
       <c r="D46" s="3"/>
@@ -6809,7 +6822,7 @@
     </row>
     <row r="47" spans="1:5" customFormat="1">
       <c r="A47" s="3"/>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="16" t="s">
         <v>551</v>
       </c>
       <c r="D47" s="3"/>
@@ -6817,7 +6830,7 @@
     </row>
     <row r="48" spans="1:5" customFormat="1">
       <c r="A48" s="3"/>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>552</v>
       </c>
       <c r="D48" s="3"/>
@@ -6825,7 +6838,7 @@
     </row>
     <row r="49" spans="1:5" customFormat="1">
       <c r="A49" s="3"/>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="17" t="s">
         <v>553</v>
       </c>
       <c r="D49" s="3"/>
@@ -6833,7 +6846,7 @@
     </row>
     <row r="50" spans="1:5" customFormat="1">
       <c r="A50" s="3"/>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="17" t="s">
         <v>554</v>
       </c>
       <c r="D50" s="3"/>
@@ -6841,7 +6854,7 @@
     </row>
     <row r="51" spans="1:5" customFormat="1">
       <c r="A51" s="3"/>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="17" t="s">
         <v>555</v>
       </c>
       <c r="D51" s="3"/>
@@ -6849,7 +6862,7 @@
     </row>
     <row r="52" spans="1:5" customFormat="1">
       <c r="A52" s="3"/>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="16" t="s">
         <v>556</v>
       </c>
       <c r="D52" s="3"/>
@@ -6857,7 +6870,7 @@
     </row>
     <row r="53" spans="1:5" customFormat="1" ht="26.4">
       <c r="A53" s="3"/>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="17" t="s">
         <v>557</v>
       </c>
       <c r="D53" s="3"/>
@@ -6865,7 +6878,7 @@
     </row>
     <row r="54" spans="1:5" customFormat="1">
       <c r="A54" s="3"/>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="17" t="s">
         <v>558</v>
       </c>
       <c r="D54" s="3"/>
@@ -6873,7 +6886,7 @@
     </row>
     <row r="55" spans="1:5" customFormat="1">
       <c r="A55" s="3"/>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="17" t="s">
         <v>559</v>
       </c>
       <c r="D55" s="3"/>
@@ -6881,7 +6894,7 @@
     </row>
     <row r="56" spans="1:5" customFormat="1">
       <c r="A56" s="3"/>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="17" t="s">
         <v>560</v>
       </c>
       <c r="D56" s="3"/>
@@ -6889,7 +6902,7 @@
     </row>
     <row r="57" spans="1:5" customFormat="1">
       <c r="A57" s="3"/>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="16" t="s">
         <v>561</v>
       </c>
       <c r="D57" s="3"/>
@@ -6897,7 +6910,7 @@
     </row>
     <row r="58" spans="1:5" customFormat="1">
       <c r="A58" s="3"/>
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="17" t="s">
         <v>562</v>
       </c>
       <c r="D58" s="3"/>
@@ -6905,7 +6918,7 @@
     </row>
     <row r="59" spans="1:5" customFormat="1">
       <c r="A59" s="3"/>
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="17" t="s">
         <v>563</v>
       </c>
       <c r="D59" s="3"/>
@@ -6913,7 +6926,7 @@
     </row>
     <row r="60" spans="1:5" customFormat="1">
       <c r="A60" s="3"/>
-      <c r="B60" s="18" t="s">
+      <c r="B60" s="17" t="s">
         <v>564</v>
       </c>
       <c r="D60" s="3"/>
@@ -6921,7 +6934,7 @@
     </row>
     <row r="61" spans="1:5" customFormat="1">
       <c r="A61" s="3"/>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="17" t="s">
         <v>565</v>
       </c>
       <c r="D61" s="3"/>
@@ -6929,7 +6942,7 @@
     </row>
     <row r="62" spans="1:5" customFormat="1">
       <c r="A62" s="3"/>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="16" t="s">
         <v>566</v>
       </c>
       <c r="D62" s="3"/>
@@ -6937,7 +6950,7 @@
     </row>
     <row r="63" spans="1:5" customFormat="1" ht="26.4">
       <c r="A63" s="3"/>
-      <c r="B63" s="18" t="s">
+      <c r="B63" s="17" t="s">
         <v>567</v>
       </c>
       <c r="D63" s="3"/>
@@ -6945,7 +6958,7 @@
     </row>
     <row r="64" spans="1:5" customFormat="1">
       <c r="A64" s="3"/>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="17" t="s">
         <v>568</v>
       </c>
       <c r="D64" s="3"/>
@@ -6953,7 +6966,7 @@
     </row>
     <row r="65" spans="1:5" customFormat="1">
       <c r="A65" s="3"/>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="17" t="s">
         <v>569</v>
       </c>
       <c r="D65" s="3"/>
@@ -6961,7 +6974,7 @@
     </row>
     <row r="66" spans="1:5" customFormat="1">
       <c r="A66" s="3"/>
-      <c r="B66" s="18" t="s">
+      <c r="B66" s="17" t="s">
         <v>570</v>
       </c>
       <c r="D66" s="3"/>
@@ -6969,7 +6982,7 @@
     </row>
     <row r="67" spans="1:5" customFormat="1">
       <c r="A67" s="3"/>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="16" t="s">
         <v>571</v>
       </c>
       <c r="D67" s="3"/>
@@ -6977,7 +6990,7 @@
     </row>
     <row r="68" spans="1:5" customFormat="1">
       <c r="A68" s="3"/>
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="17" t="s">
         <v>572</v>
       </c>
       <c r="D68" s="3"/>
@@ -6985,7 +6998,7 @@
     </row>
     <row r="69" spans="1:5" customFormat="1">
       <c r="A69" s="3"/>
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="17" t="s">
         <v>573</v>
       </c>
       <c r="D69" s="3"/>
@@ -6993,7 +7006,7 @@
     </row>
     <row r="70" spans="1:5" customFormat="1">
       <c r="A70" s="3"/>
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="17" t="s">
         <v>574</v>
       </c>
       <c r="D70" s="3"/>
@@ -7001,7 +7014,7 @@
     </row>
     <row r="71" spans="1:5" customFormat="1">
       <c r="A71" s="3"/>
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="17" t="s">
         <v>575</v>
       </c>
       <c r="D71" s="3"/>
@@ -7009,7 +7022,7 @@
     </row>
     <row r="72" spans="1:5" customFormat="1">
       <c r="A72" s="3"/>
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="16" t="s">
         <v>576</v>
       </c>
       <c r="D72" s="3"/>
@@ -7017,7 +7030,7 @@
     </row>
     <row r="73" spans="1:5" customFormat="1">
       <c r="A73" s="3"/>
-      <c r="B73" s="18" t="s">
+      <c r="B73" s="17" t="s">
         <v>577</v>
       </c>
       <c r="D73" s="3"/>
@@ -7025,7 +7038,7 @@
     </row>
     <row r="74" spans="1:5" customFormat="1">
       <c r="A74" s="3"/>
-      <c r="B74" s="18" t="s">
+      <c r="B74" s="17" t="s">
         <v>578</v>
       </c>
       <c r="D74" s="3"/>
@@ -7033,7 +7046,7 @@
     </row>
     <row r="75" spans="1:5" customFormat="1">
       <c r="A75" s="3"/>
-      <c r="B75" s="18" t="s">
+      <c r="B75" s="17" t="s">
         <v>579</v>
       </c>
       <c r="D75" s="3"/>
@@ -7041,7 +7054,7 @@
     </row>
     <row r="76" spans="1:5" customFormat="1">
       <c r="A76" s="3"/>
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="17" t="s">
         <v>580</v>
       </c>
       <c r="D76" s="3"/>
@@ -7049,7 +7062,7 @@
     </row>
     <row r="77" spans="1:5" customFormat="1">
       <c r="A77" s="3"/>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="16" t="s">
         <v>581</v>
       </c>
       <c r="D77" s="3"/>
@@ -7057,7 +7070,7 @@
     </row>
     <row r="78" spans="1:5" customFormat="1">
       <c r="A78" s="3"/>
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="17" t="s">
         <v>582</v>
       </c>
       <c r="D78" s="3"/>
@@ -7065,7 +7078,7 @@
     </row>
     <row r="79" spans="1:5" customFormat="1">
       <c r="A79" s="3"/>
-      <c r="B79" s="18" t="s">
+      <c r="B79" s="17" t="s">
         <v>583</v>
       </c>
       <c r="D79" s="3"/>
@@ -7073,14 +7086,14 @@
     </row>
     <row r="80" spans="1:5" customFormat="1">
       <c r="A80" s="3"/>
-      <c r="B80" s="18" t="s">
+      <c r="B80" s="17" t="s">
         <v>584</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="18" t="s">
+      <c r="B81" s="17" t="s">
         <v>585</v>
       </c>
     </row>
@@ -7095,7 +7108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8A1622-8C2E-411B-B665-598CD679D319}">
   <dimension ref="A1:E271"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -7110,218 +7123,218 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="13.8">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="2:5" ht="13.8">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>586</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="13.8">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>587</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" ht="13.8">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>588</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="13.8">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>589</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="13.8">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="2:5" ht="13.8">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>591</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="2:5" ht="13.8">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="2:5" ht="13.8">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="2:5" ht="13.8">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="2:5" ht="13.8">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="2:5" ht="13.8">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>596</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="2:5" ht="13.8">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="2:5" ht="13.8">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>598</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="2:5" ht="13.8">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>599</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="2:5" ht="13.8">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>600</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="26.4">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>601</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" ht="13.8">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>602</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="13.8">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>603</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" ht="13.8">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22" t="s">
         <v>604</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="21" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="26.4">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="21" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="22" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="31" spans="1:5" customFormat="1">
       <c r="A31" s="3"/>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="22" t="s">
         <v>615</v>
       </c>
       <c r="D31" s="3"/>
@@ -7329,7 +7342,7 @@
     </row>
     <row r="32" spans="1:5" customFormat="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>616</v>
       </c>
       <c r="D32" s="3"/>
@@ -7337,7 +7350,7 @@
     </row>
     <row r="33" spans="1:5" customFormat="1">
       <c r="A33" s="3"/>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="22" t="s">
         <v>617</v>
       </c>
       <c r="D33" s="3"/>
@@ -7345,7 +7358,7 @@
     </row>
     <row r="34" spans="1:5" customFormat="1">
       <c r="A34" s="3"/>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="22" t="s">
         <v>618</v>
       </c>
       <c r="D34" s="3"/>
@@ -7353,7 +7366,7 @@
     </row>
     <row r="35" spans="1:5" customFormat="1">
       <c r="A35" s="3"/>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="22" t="s">
         <v>619</v>
       </c>
       <c r="D35" s="3"/>
@@ -7361,7 +7374,7 @@
     </row>
     <row r="36" spans="1:5" customFormat="1">
       <c r="A36" s="3"/>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="22" t="s">
         <v>620</v>
       </c>
       <c r="D36" s="3"/>
@@ -7369,7 +7382,7 @@
     </row>
     <row r="37" spans="1:5" customFormat="1" ht="26.4">
       <c r="A37" s="3"/>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="21" t="s">
         <v>621</v>
       </c>
       <c r="D37" s="3"/>
@@ -7377,7 +7390,7 @@
     </row>
     <row r="38" spans="1:5" customFormat="1">
       <c r="A38" s="3"/>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="22" t="s">
         <v>622</v>
       </c>
       <c r="D38" s="3"/>
@@ -7385,7 +7398,7 @@
     </row>
     <row r="39" spans="1:5" customFormat="1">
       <c r="A39" s="3"/>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="22" t="s">
         <v>623</v>
       </c>
       <c r="D39" s="3"/>
@@ -7393,7 +7406,7 @@
     </row>
     <row r="40" spans="1:5" customFormat="1">
       <c r="A40" s="3"/>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="22" t="s">
         <v>624</v>
       </c>
       <c r="D40" s="3"/>
@@ -7401,7 +7414,7 @@
     </row>
     <row r="41" spans="1:5" customFormat="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="22" t="s">
         <v>625</v>
       </c>
       <c r="D41" s="3"/>
@@ -7409,7 +7422,7 @@
     </row>
     <row r="42" spans="1:5" customFormat="1">
       <c r="A42" s="3"/>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="21" t="s">
         <v>626</v>
       </c>
       <c r="D42" s="3"/>
@@ -7417,7 +7430,7 @@
     </row>
     <row r="43" spans="1:5" customFormat="1">
       <c r="A43" s="3"/>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="22" t="s">
         <v>627</v>
       </c>
       <c r="D43" s="3"/>
@@ -7425,7 +7438,7 @@
     </row>
     <row r="44" spans="1:5" customFormat="1">
       <c r="A44" s="3"/>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="22" t="s">
         <v>628</v>
       </c>
       <c r="D44" s="3"/>
@@ -7433,7 +7446,7 @@
     </row>
     <row r="45" spans="1:5" customFormat="1">
       <c r="A45" s="3"/>
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="22" t="s">
         <v>629</v>
       </c>
       <c r="D45" s="3"/>
@@ -7441,7 +7454,7 @@
     </row>
     <row r="46" spans="1:5" customFormat="1">
       <c r="A46" s="3"/>
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="22" t="s">
         <v>630</v>
       </c>
       <c r="D46" s="3"/>
@@ -7449,7 +7462,7 @@
     </row>
     <row r="47" spans="1:5" customFormat="1">
       <c r="A47" s="3"/>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="21" t="s">
         <v>631</v>
       </c>
       <c r="D47" s="3"/>
@@ -7457,7 +7470,7 @@
     </row>
     <row r="48" spans="1:5" customFormat="1">
       <c r="A48" s="3"/>
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="22" t="s">
         <v>632</v>
       </c>
       <c r="D48" s="3"/>
@@ -7465,7 +7478,7 @@
     </row>
     <row r="49" spans="1:5" customFormat="1">
       <c r="A49" s="3"/>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="22" t="s">
         <v>633</v>
       </c>
       <c r="D49" s="3"/>
@@ -7473,7 +7486,7 @@
     </row>
     <row r="50" spans="1:5" customFormat="1">
       <c r="A50" s="3"/>
-      <c r="B50" s="23" t="s">
+      <c r="B50" s="22" t="s">
         <v>634</v>
       </c>
       <c r="D50" s="3"/>
@@ -7481,7 +7494,7 @@
     </row>
     <row r="51" spans="1:5" customFormat="1" ht="26.4">
       <c r="A51" s="3"/>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="22" t="s">
         <v>635</v>
       </c>
       <c r="D51" s="3"/>
@@ -7489,7 +7502,7 @@
     </row>
     <row r="52" spans="1:5" customFormat="1" ht="26.4">
       <c r="A52" s="3"/>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="21" t="s">
         <v>636</v>
       </c>
       <c r="D52" s="3"/>
@@ -7497,7 +7510,7 @@
     </row>
     <row r="53" spans="1:5" customFormat="1">
       <c r="A53" s="3"/>
-      <c r="B53" s="23" t="s">
+      <c r="B53" s="22" t="s">
         <v>637</v>
       </c>
       <c r="D53" s="3"/>
@@ -7505,7 +7518,7 @@
     </row>
     <row r="54" spans="1:5" customFormat="1">
       <c r="A54" s="3"/>
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="22" t="s">
         <v>638</v>
       </c>
       <c r="D54" s="3"/>
@@ -7513,7 +7526,7 @@
     </row>
     <row r="55" spans="1:5" customFormat="1">
       <c r="A55" s="3"/>
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="22" t="s">
         <v>639</v>
       </c>
       <c r="D55" s="3"/>
@@ -7521,7 +7534,7 @@
     </row>
     <row r="56" spans="1:5" customFormat="1">
       <c r="A56" s="3"/>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="22" t="s">
         <v>640</v>
       </c>
       <c r="D56" s="3"/>
@@ -7529,7 +7542,7 @@
     </row>
     <row r="57" spans="1:5" customFormat="1">
       <c r="A57" s="3"/>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="21" t="s">
         <v>641</v>
       </c>
       <c r="D57" s="3"/>
@@ -7537,7 +7550,7 @@
     </row>
     <row r="58" spans="1:5" customFormat="1">
       <c r="A58" s="3"/>
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="22" t="s">
         <v>642</v>
       </c>
       <c r="D58" s="3"/>
@@ -7545,7 +7558,7 @@
     </row>
     <row r="59" spans="1:5" customFormat="1">
       <c r="A59" s="3"/>
-      <c r="B59" s="23" t="s">
+      <c r="B59" s="22" t="s">
         <v>643</v>
       </c>
       <c r="D59" s="3"/>
@@ -7553,7 +7566,7 @@
     </row>
     <row r="60" spans="1:5" customFormat="1">
       <c r="A60" s="3"/>
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="22" t="s">
         <v>644</v>
       </c>
       <c r="D60" s="3"/>
@@ -7561,7 +7574,7 @@
     </row>
     <row r="61" spans="1:5" customFormat="1">
       <c r="A61" s="3"/>
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="22" t="s">
         <v>645</v>
       </c>
       <c r="D61" s="3"/>
@@ -7569,7 +7582,7 @@
     </row>
     <row r="62" spans="1:5" customFormat="1">
       <c r="A62" s="3"/>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="21" t="s">
         <v>646</v>
       </c>
       <c r="D62" s="3"/>
@@ -7577,7 +7590,7 @@
     </row>
     <row r="63" spans="1:5" customFormat="1">
       <c r="A63" s="3"/>
-      <c r="B63" s="23" t="s">
+      <c r="B63" s="22" t="s">
         <v>647</v>
       </c>
       <c r="D63" s="3"/>
@@ -7585,7 +7598,7 @@
     </row>
     <row r="64" spans="1:5" customFormat="1">
       <c r="A64" s="3"/>
-      <c r="B64" s="23" t="s">
+      <c r="B64" s="22" t="s">
         <v>648</v>
       </c>
       <c r="D64" s="3"/>
@@ -7593,7 +7606,7 @@
     </row>
     <row r="65" spans="1:5" customFormat="1">
       <c r="A65" s="3"/>
-      <c r="B65" s="23" t="s">
+      <c r="B65" s="22" t="s">
         <v>649</v>
       </c>
       <c r="D65" s="3"/>
@@ -7601,7 +7614,7 @@
     </row>
     <row r="66" spans="1:5" customFormat="1">
       <c r="A66" s="3"/>
-      <c r="B66" s="23" t="s">
+      <c r="B66" s="22" t="s">
         <v>650</v>
       </c>
       <c r="D66" s="3"/>
@@ -7609,7 +7622,7 @@
     </row>
     <row r="67" spans="1:5" customFormat="1" ht="52.8">
       <c r="A67" s="3"/>
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="21" t="s">
         <v>651</v>
       </c>
       <c r="D67" s="3"/>
@@ -7617,7 +7630,7 @@
     </row>
     <row r="68" spans="1:5" customFormat="1">
       <c r="A68" s="3"/>
-      <c r="B68" s="23" t="s">
+      <c r="B68" s="22" t="s">
         <v>652</v>
       </c>
       <c r="D68" s="3"/>
@@ -7625,7 +7638,7 @@
     </row>
     <row r="69" spans="1:5" customFormat="1">
       <c r="A69" s="3"/>
-      <c r="B69" s="23" t="s">
+      <c r="B69" s="22" t="s">
         <v>653</v>
       </c>
       <c r="D69" s="3"/>
@@ -7633,7 +7646,7 @@
     </row>
     <row r="70" spans="1:5" customFormat="1">
       <c r="A70" s="3"/>
-      <c r="B70" s="23" t="s">
+      <c r="B70" s="22" t="s">
         <v>654</v>
       </c>
       <c r="D70" s="3"/>
@@ -7641,7 +7654,7 @@
     </row>
     <row r="71" spans="1:5" customFormat="1">
       <c r="A71" s="3"/>
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="22" t="s">
         <v>655</v>
       </c>
       <c r="D71" s="3"/>
@@ -7649,7 +7662,7 @@
     </row>
     <row r="72" spans="1:5" customFormat="1">
       <c r="A72" s="3"/>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="21" t="s">
         <v>656</v>
       </c>
       <c r="D72" s="3"/>
@@ -7657,7 +7670,7 @@
     </row>
     <row r="73" spans="1:5" customFormat="1">
       <c r="A73" s="3"/>
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="22" t="s">
         <v>657</v>
       </c>
       <c r="D73" s="3"/>
@@ -7665,7 +7678,7 @@
     </row>
     <row r="74" spans="1:5" customFormat="1">
       <c r="A74" s="3"/>
-      <c r="B74" s="23" t="s">
+      <c r="B74" s="22" t="s">
         <v>658</v>
       </c>
       <c r="D74" s="3"/>
@@ -7673,7 +7686,7 @@
     </row>
     <row r="75" spans="1:5" customFormat="1">
       <c r="A75" s="3"/>
-      <c r="B75" s="23" t="s">
+      <c r="B75" s="22" t="s">
         <v>659</v>
       </c>
       <c r="D75" s="3"/>
@@ -7681,7 +7694,7 @@
     </row>
     <row r="76" spans="1:5" customFormat="1">
       <c r="A76" s="3"/>
-      <c r="B76" s="23" t="s">
+      <c r="B76" s="22" t="s">
         <v>660</v>
       </c>
       <c r="D76" s="3"/>
@@ -7689,7 +7702,7 @@
     </row>
     <row r="77" spans="1:5" customFormat="1">
       <c r="A77" s="3"/>
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="21" t="s">
         <v>661</v>
       </c>
       <c r="D77" s="3"/>
@@ -7697,7 +7710,7 @@
     </row>
     <row r="78" spans="1:5" customFormat="1" ht="26.4">
       <c r="A78" s="3"/>
-      <c r="B78" s="23" t="s">
+      <c r="B78" s="22" t="s">
         <v>662</v>
       </c>
       <c r="D78" s="3"/>
@@ -7705,7 +7718,7 @@
     </row>
     <row r="79" spans="1:5" customFormat="1" ht="26.4">
       <c r="A79" s="3"/>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="22" t="s">
         <v>663</v>
       </c>
       <c r="D79" s="3"/>
@@ -7713,964 +7726,964 @@
     </row>
     <row r="80" spans="1:5" customFormat="1" ht="26.4">
       <c r="A80" s="3"/>
-      <c r="B80" s="23" t="s">
+      <c r="B80" s="22" t="s">
         <v>664</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="23" t="s">
+      <c r="B81" s="22" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="26.4">
-      <c r="B82" s="22" t="s">
+      <c r="B82" s="21" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="23" t="s">
+      <c r="B83" s="22" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="23" t="s">
+      <c r="B84" s="22" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="23" t="s">
+      <c r="B85" s="22" t="s">
         <v>669</v>
       </c>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="22" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="87" spans="2:2" ht="26.4">
-      <c r="B87" s="22" t="s">
+      <c r="B87" s="21" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="23" t="s">
+      <c r="B88" s="22" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="23" t="s">
+      <c r="B89" s="22" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="23" t="s">
+      <c r="B90" s="22" t="s">
         <v>674</v>
       </c>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="23" t="s">
+      <c r="B91" s="22" t="s">
         <v>675</v>
       </c>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="22" t="s">
+      <c r="B92" s="21" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="23" t="s">
+      <c r="B93" s="22" t="s">
         <v>677</v>
       </c>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="23" t="s">
+      <c r="B94" s="22" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="23" t="s">
+      <c r="B95" s="22" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="23" t="s">
+      <c r="B96" s="22" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="26.4">
-      <c r="B97" s="22" t="s">
+      <c r="B97" s="21" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="23" t="s">
+      <c r="B98" s="22" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="23" t="s">
+      <c r="B99" s="22" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="23" t="s">
+      <c r="B100" s="22" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="23" t="s">
+      <c r="B101" s="22" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="102" spans="2:2" ht="26.4">
-      <c r="B102" s="22" t="s">
+      <c r="B102" s="21" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="103" spans="2:2" ht="26.4">
-      <c r="B103" s="23" t="s">
+      <c r="B103" s="22" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="23" t="s">
+      <c r="B104" s="22" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="105" spans="2:2">
-      <c r="B105" s="23" t="s">
+      <c r="B105" s="22" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="106" spans="2:2" ht="26.4">
-      <c r="B106" s="23" t="s">
+      <c r="B106" s="22" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="22" t="s">
+      <c r="B107" s="21" t="s">
         <v>691</v>
       </c>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="23" t="s">
+      <c r="B108" s="22" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="23" t="s">
+      <c r="B109" s="22" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="23" t="s">
+      <c r="B110" s="22" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="23" t="s">
+      <c r="B111" s="22" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="22" t="s">
+      <c r="B112" s="21" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="23" t="s">
+      <c r="B113" s="22" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="23" t="s">
+      <c r="B114" s="22" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="23" t="s">
+      <c r="B115" s="22" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="23" t="s">
+      <c r="B116" s="22" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="117" spans="2:2" ht="26.4">
-      <c r="B117" s="22" t="s">
+      <c r="B117" s="21" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="23" t="s">
+      <c r="B118" s="22" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="23" t="s">
+      <c r="B119" s="22" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="23" t="s">
+      <c r="B120" s="22" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="23" t="s">
+      <c r="B121" s="22" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="122" spans="2:2" ht="39.6">
-      <c r="B122" s="22" t="s">
+      <c r="B122" s="21" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="23" t="s">
+      <c r="B123" s="22" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="23" t="s">
+      <c r="B124" s="22" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="23" t="s">
+      <c r="B125" s="22" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="23" t="s">
+      <c r="B126" s="22" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="22" t="s">
+      <c r="B127" s="21" t="s">
         <v>707</v>
       </c>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="23" t="s">
+      <c r="B128" s="22" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="23" t="s">
+      <c r="B129" s="22" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="23" t="s">
+      <c r="B130" s="22" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="23" t="s">
+      <c r="B131" s="22" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="22" t="s">
+      <c r="B132" s="21" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="23" t="s">
+      <c r="B133" s="22" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="23" t="s">
+      <c r="B134" s="22" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="23" t="s">
+      <c r="B135" s="22" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="23" t="s">
+      <c r="B136" s="22" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="22" t="s">
+      <c r="B137" s="21" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="23" t="s">
+      <c r="B138" s="22" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="139" spans="2:2">
-      <c r="B139" s="23" t="s">
+      <c r="B139" s="22" t="s">
         <v>719</v>
       </c>
     </row>
     <row r="140" spans="2:2">
-      <c r="B140" s="23" t="s">
+      <c r="B140" s="22" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="141" spans="2:2">
-      <c r="B141" s="23" t="s">
+      <c r="B141" s="22" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="142" spans="2:2" ht="26.4">
-      <c r="B142" s="22" t="s">
+      <c r="B142" s="21" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="143" spans="2:2">
-      <c r="B143" s="23" t="s">
+      <c r="B143" s="22" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="23" t="s">
+      <c r="B144" s="22" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="26.4">
-      <c r="B145" s="23" t="s">
+      <c r="B145" s="22" t="s">
         <v>725</v>
       </c>
     </row>
     <row r="146" spans="2:2">
-      <c r="B146" s="23" t="s">
+      <c r="B146" s="22" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="147" spans="2:2">
-      <c r="B147" s="22" t="s">
+      <c r="B147" s="21" t="s">
         <v>727</v>
       </c>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="23" t="s">
+      <c r="B148" s="22" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="149" spans="2:2">
-      <c r="B149" s="23" t="s">
+      <c r="B149" s="22" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="150" spans="2:2">
-      <c r="B150" s="23" t="s">
+      <c r="B150" s="22" t="s">
         <v>730</v>
       </c>
     </row>
     <row r="151" spans="2:2">
-      <c r="B151" s="23" t="s">
+      <c r="B151" s="22" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="152" spans="2:2" ht="26.4">
-      <c r="B152" s="22" t="s">
+      <c r="B152" s="21" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="153" spans="2:2">
-      <c r="B153" s="23" t="s">
+      <c r="B153" s="22" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="154" spans="2:2">
-      <c r="B154" s="23" t="s">
+      <c r="B154" s="22" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="155" spans="2:2">
-      <c r="B155" s="23" t="s">
+      <c r="B155" s="22" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="156" spans="2:2">
-      <c r="B156" s="23" t="s">
+      <c r="B156" s="22" t="s">
         <v>736</v>
       </c>
     </row>
     <row r="157" spans="2:2" ht="26.4">
-      <c r="B157" s="22" t="s">
+      <c r="B157" s="21" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="158" spans="2:2">
-      <c r="B158" s="23" t="s">
+      <c r="B158" s="22" t="s">
         <v>738</v>
       </c>
     </row>
     <row r="159" spans="2:2">
-      <c r="B159" s="23" t="s">
+      <c r="B159" s="22" t="s">
         <v>739</v>
       </c>
     </row>
     <row r="160" spans="2:2">
-      <c r="B160" s="23" t="s">
+      <c r="B160" s="22" t="s">
         <v>740</v>
       </c>
     </row>
     <row r="161" spans="2:2">
-      <c r="B161" s="23" t="s">
+      <c r="B161" s="22" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="162" spans="2:2" ht="26.4">
-      <c r="B162" s="22" t="s">
+      <c r="B162" s="21" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="163" spans="2:2">
-      <c r="B163" s="23" t="s">
+      <c r="B163" s="22" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="164" spans="2:2">
-      <c r="B164" s="23" t="s">
+      <c r="B164" s="22" t="s">
         <v>744</v>
       </c>
     </row>
     <row r="165" spans="2:2">
-      <c r="B165" s="23" t="s">
+      <c r="B165" s="22" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="166" spans="2:2">
-      <c r="B166" s="23" t="s">
+      <c r="B166" s="22" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="167" spans="2:2" ht="26.4">
-      <c r="B167" s="22" t="s">
+      <c r="B167" s="21" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="168" spans="2:2">
-      <c r="B168" s="23" t="s">
+      <c r="B168" s="22" t="s">
         <v>748</v>
       </c>
     </row>
     <row r="169" spans="2:2">
-      <c r="B169" s="23" t="s">
+      <c r="B169" s="22" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="170" spans="2:2">
-      <c r="B170" s="23" t="s">
+      <c r="B170" s="22" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="171" spans="2:2">
-      <c r="B171" s="23" t="s">
+      <c r="B171" s="22" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="172" spans="2:2">
-      <c r="B172" s="22" t="s">
+      <c r="B172" s="21" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="173" spans="2:2">
-      <c r="B173" s="23" t="s">
+      <c r="B173" s="22" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="174" spans="2:2">
-      <c r="B174" s="23" t="s">
+      <c r="B174" s="22" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="175" spans="2:2">
-      <c r="B175" s="23" t="s">
+      <c r="B175" s="22" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="176" spans="2:2">
-      <c r="B176" s="23" t="s">
+      <c r="B176" s="22" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="177" spans="2:2" ht="26.4">
-      <c r="B177" s="22" t="s">
+      <c r="B177" s="21" t="s">
         <v>757</v>
       </c>
     </row>
     <row r="178" spans="2:2">
-      <c r="B178" s="23" t="s">
+      <c r="B178" s="22" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="179" spans="2:2">
-      <c r="B179" s="23" t="s">
+      <c r="B179" s="22" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="180" spans="2:2">
-      <c r="B180" s="23" t="s">
+      <c r="B180" s="22" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="181" spans="2:2">
-      <c r="B181" s="23" t="s">
+      <c r="B181" s="22" t="s">
         <v>761</v>
       </c>
     </row>
     <row r="182" spans="2:2">
-      <c r="B182" s="22" t="s">
+      <c r="B182" s="21" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="183" spans="2:2">
-      <c r="B183" s="23" t="s">
+      <c r="B183" s="22" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="184" spans="2:2">
-      <c r="B184" s="23" t="s">
+      <c r="B184" s="22" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="185" spans="2:2">
-      <c r="B185" s="23" t="s">
+      <c r="B185" s="22" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="186" spans="2:2">
-      <c r="B186" s="23" t="s">
+      <c r="B186" s="22" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="187" spans="2:2" ht="26.4">
-      <c r="B187" s="22" t="s">
+      <c r="B187" s="21" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="188" spans="2:2">
-      <c r="B188" s="23" t="s">
+      <c r="B188" s="22" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="189" spans="2:2">
-      <c r="B189" s="23" t="s">
+      <c r="B189" s="22" t="s">
         <v>769</v>
       </c>
     </row>
     <row r="190" spans="2:2">
-      <c r="B190" s="23" t="s">
+      <c r="B190" s="22" t="s">
         <v>770</v>
       </c>
     </row>
     <row r="191" spans="2:2">
-      <c r="B191" s="23" t="s">
+      <c r="B191" s="22" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="192" spans="2:2" ht="26.4">
-      <c r="B192" s="22" t="s">
+      <c r="B192" s="21" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="193" spans="2:2">
-      <c r="B193" s="23" t="s">
+      <c r="B193" s="22" t="s">
         <v>773</v>
       </c>
     </row>
     <row r="194" spans="2:2">
-      <c r="B194" s="23" t="s">
+      <c r="B194" s="22" t="s">
         <v>774</v>
       </c>
     </row>
     <row r="195" spans="2:2">
-      <c r="B195" s="23" t="s">
+      <c r="B195" s="22" t="s">
         <v>775</v>
       </c>
     </row>
     <row r="196" spans="2:2">
-      <c r="B196" s="23" t="s">
+      <c r="B196" s="22" t="s">
         <v>776</v>
       </c>
     </row>
     <row r="197" spans="2:2" ht="26.4">
-      <c r="B197" s="22" t="s">
+      <c r="B197" s="21" t="s">
         <v>777</v>
       </c>
     </row>
     <row r="198" spans="2:2">
-      <c r="B198" s="23" t="s">
+      <c r="B198" s="22" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="199" spans="2:2">
-      <c r="B199" s="23" t="s">
+      <c r="B199" s="22" t="s">
         <v>779</v>
       </c>
     </row>
     <row r="200" spans="2:2">
-      <c r="B200" s="23" t="s">
+      <c r="B200" s="22" t="s">
         <v>780</v>
       </c>
     </row>
     <row r="201" spans="2:2">
-      <c r="B201" s="23" t="s">
+      <c r="B201" s="22" t="s">
         <v>781</v>
       </c>
     </row>
     <row r="202" spans="2:2">
-      <c r="B202" s="22" t="s">
+      <c r="B202" s="21" t="s">
         <v>782</v>
       </c>
     </row>
     <row r="203" spans="2:2">
-      <c r="B203" s="23" t="s">
+      <c r="B203" s="22" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="204" spans="2:2">
-      <c r="B204" s="23" t="s">
+      <c r="B204" s="22" t="s">
         <v>784</v>
       </c>
     </row>
     <row r="205" spans="2:2">
-      <c r="B205" s="23" t="s">
+      <c r="B205" s="22" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="206" spans="2:2">
-      <c r="B206" s="23" t="s">
+      <c r="B206" s="22" t="s">
         <v>786</v>
       </c>
     </row>
     <row r="207" spans="2:2">
-      <c r="B207" s="22" t="s">
+      <c r="B207" s="21" t="s">
         <v>787</v>
       </c>
     </row>
     <row r="208" spans="2:2">
-      <c r="B208" s="23" t="s">
+      <c r="B208" s="22" t="s">
         <v>788</v>
       </c>
     </row>
     <row r="209" spans="2:2">
-      <c r="B209" s="23" t="s">
+      <c r="B209" s="22" t="s">
         <v>789</v>
       </c>
     </row>
     <row r="210" spans="2:2">
-      <c r="B210" s="23" t="s">
+      <c r="B210" s="22" t="s">
         <v>790</v>
       </c>
     </row>
     <row r="211" spans="2:2">
-      <c r="B211" s="23" t="s">
+      <c r="B211" s="22" t="s">
         <v>791</v>
       </c>
     </row>
     <row r="212" spans="2:2" ht="26.4">
-      <c r="B212" s="22" t="s">
+      <c r="B212" s="21" t="s">
         <v>792</v>
       </c>
     </row>
     <row r="213" spans="2:2">
-      <c r="B213" s="23" t="s">
+      <c r="B213" s="22" t="s">
         <v>793</v>
       </c>
     </row>
     <row r="214" spans="2:2">
-      <c r="B214" s="23" t="s">
+      <c r="B214" s="22" t="s">
         <v>794</v>
       </c>
     </row>
     <row r="215" spans="2:2">
-      <c r="B215" s="23" t="s">
+      <c r="B215" s="22" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="216" spans="2:2">
-      <c r="B216" s="23" t="s">
+      <c r="B216" s="22" t="s">
         <v>796</v>
       </c>
     </row>
     <row r="217" spans="2:2">
-      <c r="B217" s="22" t="s">
+      <c r="B217" s="21" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="218" spans="2:2">
-      <c r="B218" s="23" t="s">
+      <c r="B218" s="22" t="s">
         <v>798</v>
       </c>
     </row>
     <row r="219" spans="2:2">
-      <c r="B219" s="23" t="s">
+      <c r="B219" s="22" t="s">
         <v>799</v>
       </c>
     </row>
     <row r="220" spans="2:2">
-      <c r="B220" s="23" t="s">
+      <c r="B220" s="22" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="221" spans="2:2">
-      <c r="B221" s="23" t="s">
+      <c r="B221" s="22" t="s">
         <v>801</v>
       </c>
     </row>
     <row r="222" spans="2:2" ht="26.4">
-      <c r="B222" s="22" t="s">
+      <c r="B222" s="21" t="s">
         <v>802</v>
       </c>
     </row>
     <row r="223" spans="2:2">
-      <c r="B223" s="23" t="s">
+      <c r="B223" s="22" t="s">
         <v>803</v>
       </c>
     </row>
     <row r="224" spans="2:2">
-      <c r="B224" s="23" t="s">
+      <c r="B224" s="22" t="s">
         <v>804</v>
       </c>
     </row>
     <row r="225" spans="2:2">
-      <c r="B225" s="23" t="s">
+      <c r="B225" s="22" t="s">
         <v>805</v>
       </c>
     </row>
     <row r="226" spans="2:2">
-      <c r="B226" s="23" t="s">
+      <c r="B226" s="22" t="s">
         <v>806</v>
       </c>
     </row>
     <row r="227" spans="2:2" ht="26.4">
-      <c r="B227" s="22" t="s">
+      <c r="B227" s="21" t="s">
         <v>807</v>
       </c>
     </row>
     <row r="228" spans="2:2">
-      <c r="B228" s="23" t="s">
+      <c r="B228" s="22" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="229" spans="2:2">
-      <c r="B229" s="23" t="s">
+      <c r="B229" s="22" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="230" spans="2:2">
-      <c r="B230" s="23" t="s">
+      <c r="B230" s="22" t="s">
         <v>810</v>
       </c>
     </row>
     <row r="231" spans="2:2">
-      <c r="B231" s="23" t="s">
+      <c r="B231" s="22" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="232" spans="2:2">
-      <c r="B232" s="22" t="s">
+      <c r="B232" s="21" t="s">
         <v>812</v>
       </c>
     </row>
     <row r="233" spans="2:2">
-      <c r="B233" s="23" t="s">
+      <c r="B233" s="22" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="234" spans="2:2">
-      <c r="B234" s="23" t="s">
+      <c r="B234" s="22" t="s">
         <v>814</v>
       </c>
     </row>
     <row r="235" spans="2:2">
-      <c r="B235" s="23" t="s">
+      <c r="B235" s="22" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="236" spans="2:2">
-      <c r="B236" s="23" t="s">
+      <c r="B236" s="22" t="s">
         <v>816</v>
       </c>
     </row>
     <row r="237" spans="2:2">
-      <c r="B237" s="22" t="s">
+      <c r="B237" s="21" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="238" spans="2:2" ht="26.4">
-      <c r="B238" s="23" t="s">
+      <c r="B238" s="22" t="s">
         <v>818</v>
       </c>
     </row>
     <row r="239" spans="2:2">
-      <c r="B239" s="23" t="s">
+      <c r="B239" s="22" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="240" spans="2:2">
-      <c r="B240" s="23" t="s">
+      <c r="B240" s="22" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="241" spans="2:2">
-      <c r="B241" s="23" t="s">
+      <c r="B241" s="22" t="s">
         <v>821</v>
       </c>
     </row>
     <row r="242" spans="2:2" ht="26.4">
-      <c r="B242" s="22" t="s">
+      <c r="B242" s="21" t="s">
         <v>822</v>
       </c>
     </row>
     <row r="243" spans="2:2">
-      <c r="B243" s="23" t="s">
+      <c r="B243" s="22" t="s">
         <v>823</v>
       </c>
     </row>
     <row r="244" spans="2:2">
-      <c r="B244" s="23" t="s">
+      <c r="B244" s="22" t="s">
         <v>824</v>
       </c>
     </row>
     <row r="245" spans="2:2">
-      <c r="B245" s="23" t="s">
+      <c r="B245" s="22" t="s">
         <v>825</v>
       </c>
     </row>
     <row r="246" spans="2:2">
-      <c r="B246" s="23" t="s">
+      <c r="B246" s="22" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="247" spans="2:2">
-      <c r="B247" s="22" t="s">
+      <c r="B247" s="21" t="s">
         <v>827</v>
       </c>
     </row>
     <row r="248" spans="2:2">
-      <c r="B248" s="23" t="s">
+      <c r="B248" s="22" t="s">
         <v>828</v>
       </c>
     </row>
     <row r="249" spans="2:2">
-      <c r="B249" s="23" t="s">
+      <c r="B249" s="22" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="250" spans="2:2">
-      <c r="B250" s="23" t="s">
+      <c r="B250" s="22" t="s">
         <v>830</v>
       </c>
     </row>
     <row r="251" spans="2:2">
-      <c r="B251" s="23" t="s">
+      <c r="B251" s="22" t="s">
         <v>831</v>
       </c>
     </row>
     <row r="252" spans="2:2">
-      <c r="B252" s="22" t="s">
+      <c r="B252" s="21" t="s">
         <v>832</v>
       </c>
     </row>
     <row r="253" spans="2:2">
-      <c r="B253" s="23" t="s">
+      <c r="B253" s="22" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="254" spans="2:2">
-      <c r="B254" s="23" t="s">
+      <c r="B254" s="22" t="s">
         <v>834</v>
       </c>
     </row>
     <row r="255" spans="2:2">
-      <c r="B255" s="23" t="s">
+      <c r="B255" s="22" t="s">
         <v>835</v>
       </c>
     </row>
     <row r="256" spans="2:2">
-      <c r="B256" s="23" t="s">
+      <c r="B256" s="22" t="s">
         <v>836</v>
       </c>
     </row>
     <row r="257" spans="2:2" ht="26.4">
-      <c r="B257" s="22" t="s">
+      <c r="B257" s="21" t="s">
         <v>837</v>
       </c>
     </row>
     <row r="258" spans="2:2">
-      <c r="B258" s="23" t="s">
+      <c r="B258" s="22" t="s">
         <v>838</v>
       </c>
     </row>
     <row r="259" spans="2:2">
-      <c r="B259" s="23" t="s">
+      <c r="B259" s="22" t="s">
         <v>839</v>
       </c>
     </row>
     <row r="260" spans="2:2">
-      <c r="B260" s="23" t="s">
+      <c r="B260" s="22" t="s">
         <v>840</v>
       </c>
     </row>
     <row r="261" spans="2:2">
-      <c r="B261" s="23" t="s">
+      <c r="B261" s="22" t="s">
         <v>841</v>
       </c>
     </row>
     <row r="262" spans="2:2">
-      <c r="B262" s="22" t="s">
+      <c r="B262" s="21" t="s">
         <v>842</v>
       </c>
     </row>
     <row r="263" spans="2:2">
-      <c r="B263" s="23" t="s">
+      <c r="B263" s="22" t="s">
         <v>843</v>
       </c>
     </row>
     <row r="264" spans="2:2">
-      <c r="B264" s="23" t="s">
+      <c r="B264" s="22" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="265" spans="2:2">
-      <c r="B265" s="23" t="s">
+      <c r="B265" s="22" t="s">
         <v>845</v>
       </c>
     </row>
     <row r="266" spans="2:2">
-      <c r="B266" s="23" t="s">
+      <c r="B266" s="22" t="s">
         <v>846</v>
       </c>
     </row>
     <row r="267" spans="2:2">
-      <c r="B267" s="22" t="s">
+      <c r="B267" s="21" t="s">
         <v>847</v>
       </c>
     </row>
     <row r="268" spans="2:2">
-      <c r="B268" s="23" t="s">
+      <c r="B268" s="22" t="s">
         <v>848</v>
       </c>
     </row>
     <row r="269" spans="2:2">
-      <c r="B269" s="23" t="s">
+      <c r="B269" s="22" t="s">
         <v>849</v>
       </c>
     </row>
     <row r="270" spans="2:2">
-      <c r="B270" s="23" t="s">
+      <c r="B270" s="22" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="271" spans="2:2">
-      <c r="B271" s="23" t="s">
+      <c r="B271" s="22" t="s">
         <v>851</v>
       </c>
     </row>

</xml_diff>